<commit_message>
Logboek + PLC TEST toegevoegd
</commit_message>
<xml_diff>
--- a/Algemeen/Logboek/Logboek Cihan Kurt.xlsx
+++ b/Algemeen/Logboek/Logboek Cihan Kurt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cihan\OneDrive - Office 365 Fontys\School\Semester 4\PTT41\Algemeen\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2B86C4-C56B-47D2-9C31-0A24E0C89F5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E13963-A2FF-4AC1-9805-C1BBD08D8184}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{1FDE790C-1098-453A-B25A-4B8D392970A4}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,20 +617,20 @@
         <v>5</v>
       </c>
       <c r="D6" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="10">
         <f xml:space="preserve"> D6 - B6 - F6</f>
-        <v>-9</v>
+        <v>5</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>5</v>
@@ -1197,21 +1197,21 @@
       </c>
       <c r="D23" s="6">
         <f>D4 + D5 + D6 + D7 + D8 + D9 + D10 + D11 + D12 + D13 + D14 + D15 + D16 + D17 + D18 + D19 + D20 + D21 + D22</f>
-        <v>29.5</v>
+        <v>44.5</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="5">
         <f>F4 + F5 + F6 + F7 + F8 + F9 + F10 + F11 + F12 + F13 + F14+ F15 + F16 + F17 + F18 + F19 + F20 + F21 + F22</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="7">
         <f xml:space="preserve"> H4 + H5 + H6 + H7 + H8 + H9 + H10 + H11 + H12 + H13 + H14 + H15 + H16 + H17 + H18 + H19 + H20 + H21 + H22</f>
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Notulen Week 12 + Logboek
Notulen week 12 + Logboek van Cihan
</commit_message>
<xml_diff>
--- a/Algemeen/Logboek/Logboek Cihan Kurt.xlsx
+++ b/Algemeen/Logboek/Logboek Cihan Kurt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cihan\OneDrive - Office 365 Fontys\School\Semester 4\PTT41\Algemeen\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C283D2A-9B4D-4D9C-A80E-6D645934F1F6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0647DED5-3602-4B37-A0B1-F2DF7BA09E58}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{1FDE790C-1098-453A-B25A-4B8D392970A4}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>5</v>
@@ -840,7 +840,7 @@
       </c>
       <c r="H12" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>5</v>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B23" s="5">
         <f>B4 + B5 + B6 + B7 + B8 + B9 + B11 + B12 + B13 + B14 + B15 + B16 + B17 + B18 + B19 + B20 + B21 + B22</f>
-        <v>56.75</v>
+        <v>65.75</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>5</v>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="H23" s="7">
         <f xml:space="preserve"> H4 + H5 + H6 + H7 + H8 + H9 + H10 + H11 + H12 + H13 + H14 + H15 + H16 + H17 + H18 + H19 + H20 + H21 + H22</f>
-        <v>30.25</v>
+        <v>21.25</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Manual + Automatic Code
Manual code af. Automatic bezig. Logboek updated
</commit_message>
<xml_diff>
--- a/Algemeen/Logboek/Logboek Cihan Kurt.xlsx
+++ b/Algemeen/Logboek/Logboek Cihan Kurt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cihan\OneDrive - Office 365 Fontys\School\Semester 4\PTT41\Algemeen\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0647DED5-3602-4B37-A0B1-F2DF7BA09E58}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A5465D-D3C7-47D5-92F8-73763B664927}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{1FDE790C-1098-453A-B25A-4B8D392970A4}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,20 +827,20 @@
         <v>5</v>
       </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="10">
         <f t="shared" si="0"/>
-        <v>-9</v>
+        <v>4.75</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>5</v>
@@ -1203,21 +1203,21 @@
       </c>
       <c r="D23" s="6">
         <f>D4 + D5 + D6 + D7 + D8 + D9 + D10 + D11 + D12 + D13 + D14 + D15 + D16 + D17 + D18 + D19 + D20 + D21 + D22</f>
-        <v>102.5</v>
+        <v>116.5</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="5">
         <f>F4 + F5 + F6 + F7 + F8 + F9 + F10 + F11 + F12 + F13 + F14+ F15 + F16 + F17 + F18 + F19 + F20 + F21 + F22</f>
-        <v>6.5</v>
+        <v>6.75</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="7">
         <f xml:space="preserve"> H4 + H5 + H6 + H7 + H8 + H9 + H10 + H11 + H12 + H13 + H14 + H15 + H16 + H17 + H18 + H19 + H20 + H21 + H22</f>
-        <v>21.25</v>
+        <v>35</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Clean up voor inlevering - Cihan
</commit_message>
<xml_diff>
--- a/Algemeen/Logboek/Logboek Cihan Kurt.xlsx
+++ b/Algemeen/Logboek/Logboek Cihan Kurt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cihan\OneDrive - Office 365 Fontys\School\Semester 4\PTT41\Algemeen\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718934D4-52E8-4855-8407-A79EAA35DA2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF535F41-104E-405E-B211-49F416E55BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9528" xr2:uid="{1FDE790C-1098-453A-B25A-4B8D392970A4}"/>
   </bookViews>
@@ -487,7 +487,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>